<commit_message>
more on main controller
</commit_message>
<xml_diff>
--- a/Docs/Vaccines Dashboard Phase 1 Data v2/Stock Management/2016_Vax_Supplied-values.xlsx
+++ b/Docs/Vaccines Dashboard Phase 1 Data v2/Stock Management/2016_Vax_Supplied-values.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="BCG" sheetId="1" r:id="rId1"/>
@@ -13,8 +13,10 @@
     <sheet name="PCV" sheetId="4" r:id="rId4"/>
     <sheet name="MEASLES" sheetId="5" r:id="rId5"/>
     <sheet name="PENTA" sheetId="6" r:id="rId6"/>
+    <sheet name="HPV" sheetId="7" r:id="rId7"/>
+    <sheet name="IPV" sheetId="8" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
 </workbook>
 </file>
 
@@ -9006,7 +9008,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X118"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
@@ -25445,4 +25447,28 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>